<commit_message>
Added script for generating test data
</commit_message>
<xml_diff>
--- a/tests/data/registered_users.xlsx
+++ b/tests/data/registered_users.xlsx
@@ -16,12 +16,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -42,14 +50,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -385,15 +396,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -406,72 +417,194 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>dhpjrvso@vgtrvvan.com</t>
+          <t>cetsbvek@vmyxalzn.com</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>LAE14Yo3</t>
+          <t>915LK2Ur</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>eopkkpqv</t>
+          <t>oqtxycgj</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>xeitgfypt@otmrnhqab.com</t>
+          <t>eotwmrjhv@tiaccgqee.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>pUGadsoUp</t>
+          <t>kOaJvHBBS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>wirrynmrm</t>
+          <t>ddotrshah</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ugizztcb@ywfuputm.com</t>
+          <t>addssx@jeftdt.com</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XlFMvwLf</t>
+          <t>7pBVRm</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>mhophdrq</t>
+          <t>jvbedq</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>fvjbaeifso@ilafkjuhlv.com</t>
+          <t>qtlmljnyzvt@ulafxwyahww.com</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>e7kTm4gnzF</t>
+          <t>KGMDsglWWc1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>acvqvlmfym</t>
+          <t>xncirpsbvby</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>rdmevr@ingsjg.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>L8gAcb</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>rgaufj</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>rdm12evr@ingsjg.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>L8gA12cb</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>rga12ufj</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>azinhdz@cmjeklf.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>bJU25Wa</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>dgglykg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>kwsxpiea@vrngtydk.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>9OgU4nxL</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>qxuecfcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>wxkklqa@rnzbgle.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>p5K5x1Q</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>vgmmybe</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>hncrcushlut@cfqqmicsczn.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>5QNoRcPQK4R</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>oeenujvywzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>xwljgviytn@thizexnaki.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>6dBVBqp3kg</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>zujlpnxecw</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added allure, new tests, auth client
</commit_message>
<xml_diff>
--- a/tests/data/registered_users.xlsx
+++ b/tests/data/registered_users.xlsx
@@ -404,7 +404,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -417,17 +417,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>wxacvq@ceepny.com</t>
+          <t>pyqelbdg@nldteery.com</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>HLYxq0</t>
+          <t>kJOixCjbu1Y</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>phkbux</t>
+          <t>ewduymhkxxz</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new tests and methods for article
</commit_message>
<xml_diff>
--- a/tests/data/registered_users.xlsx
+++ b/tests/data/registered_users.xlsx
@@ -401,7 +401,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -417,17 +417,1105 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>gmanlrra@ovvszjvz.com</t>
+          <t>cddstuzv@zxhnkdcb.com</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>XPqau5UsCbg</t>
+          <t>xcMcODPEj</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>urlmmejyovd</t>
+          <t>xkqkrbagq</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>hdeyeyin@vmifemkb.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>mayvq0F8ytr</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ucitiaxlslo</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>slsqfaip@lmonkuty.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>S2lzBiG</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ryisqwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>oabgtbgh@ovobbgws.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>7sE6wid8B</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>wdxxojxra</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>fqdqvykm@wkxqbhvy.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NxZPfGS</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>pzrfmgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>kdrunekxe@lsxwmzefq.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>6nBJa0chs</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>boofmhecb</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>tuozevefvg@btxcmscjzu.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>8rdd5h5dXj</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>qsdofxvtyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>lplozaykeha@ollyjhshhhh.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>zLVtEF1shVX</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>tzvqehrjrux</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>zyxveijp@znbpltwv.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>H3xmEY0F</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>rogqmbdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>mcipjl@zusgiw.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BdJ7Bm</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>shhoho</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>zmckhnqax@ckpditqia.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ZBavDtNrA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>xveewwqyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>asnvswnd@weceudtg.com</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>rt5COJwg6</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>bmqvucwrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>lxhbdfca@zudkaewd.com</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>o0tcjqViF</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>hwfxndbfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ebmxoig@pexbzmi.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>80BPY4J</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>kfkpqqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>bkwnzd@kuqeiq.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>7i5BMw</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>dhgwoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ktwdmetzf@vfjuehprc.com</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>43BmAmIYs</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>zjqqivntw</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>rtxknntaabk@ykwczpzzisf.com</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ApRAwhGJMrf</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>tnfknmzqurw</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>edipxkpf@eywxwjuw.com</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>gJxI6mCD</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>oqgpmnpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>fbjndqnsqb@wvrdrqbsve.com</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>C34AUhaHdP</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>mdpccwpzkr</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>wegjdscj@yfwlhodm.com</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>vPHXpMhz</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>yniqcaaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>fhzmezlvksi@ryqoxllzixr.com</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>JUEieFepv7p</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>dijdjyeglac</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>dstpomlv@qycfqzvt.com</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>iGUwTvOZ</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>bnswtoqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ssapmjtjxnh@xfhanruqpsz.com</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>qvYzYqQppKz</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>zoylniqqppd</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>mmenohhptt@zywcudmqtn.com</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>9EUS8epfVT</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ocwblniwbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>mdpiuanrwn@daurduxahg.com</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>wzE3FyxR5k</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>mfmghbugpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>plydtv@vnoxte.com</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>HWREQ7</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>egdhle</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>tyqjjsjd@enodoahm.com</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>y4r8gEYG</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>nnnfqnbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>wxrddksmmvm@hzygzrhfbfy.com</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>IkcEYZQd4yv</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>qxhxabjlwbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>jciwhexi@qjuztllm.com</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>76db5nvG</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>btepcond</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>uspmrizmjn@anoyarzgmh.com</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Y3u21ILfUH</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>sariefivdy</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>slktebiudol@jkmsxjvinrt.com</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>mPBCMHlk1fI</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ufkruiipoyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>utopbo@qnjvuw.com</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>gIHOS5</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>xlptkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>lmxbodmo@hxoitlur.com</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>sEviAZx5</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>vzkrsfoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ipuxuhliyhn@kotfbojtdhd.com</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>QggntBDW6Ms</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>fwhybbcdfwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>gpqggjdk@dgljntoq.com</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>QFGKHR28</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>bcmhthjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>nnuhkh@hkcnmg.com</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ai3O0o</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>mtwehi</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>bpkrakyev@ykjxfqarf.com</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>efYlO15G0</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>nyafawwfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ipocerx@pzjnqia.com</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ptVCh8D</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>yahcirf</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>imkhnjnb@bxvzwdhe.com</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>4r9U6OxC</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>kimrxaor</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>xmrzacz@wctgtcv.com</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>FE6tk4o</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>mzjuegd</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>outfdd@gtjjup.com</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>S7k014</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>xvtuhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>rfbdcf@nucmbn.com</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ftnUSM</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ijcqqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>uyxgtposg@zdqifbxwp.com</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>tRWLqnCqt</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>ckeeqnhas</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>txppuix@eltdzmo.com</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>p5JMTNC</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>eavuayu</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ziditpeha@zcswwrvgr.com</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>sZNXxTmzC</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>ufhoafmoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>fvgyiedqvq@wexkcedzrl.com</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>VqS0h4XuBd</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>rjgjsmefxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>klbyhcw@mqiirbx.com</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>xoTx07i</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>gcjswum</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>eettrrc@ogxcuww.com</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>GvJ0DH9</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>frrydqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>qmjcuu@hswdfd.com</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>u0nuOM</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>uxisha</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>tirotapwi@hncrrwvab.com</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>V5vDWkMbF</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>inviclwlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>fgaefhxv@lzsqykbr.com</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>BCUmRk4Zm</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>zriruwpqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>tiurpefdz@cidaifdxn.com</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SH7ugs3rH</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>leixpyrua</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>vfwmytfc@qndakoxb.com</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>X3rfvNwb</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>sqnotgky</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>xwjlyu@zekszw.com</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>We69aS</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>qlpnau</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>bnyzcq@utyzct.com</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>QbvOi5</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>yhsehh</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>mdudmpfs@jsfjznum.com</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>B3jfDtGr</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>jmjdxxgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>zpjnlrm@fagqkbr.com</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>OZXilRo</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>siwwcqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>wjijeis@jthpzig.com</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>i1k5NJT</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>kuchtwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>tjlxkai@obudoqu.com</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>u5afsW6</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>gqefkvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>mgxqaxepi@mzsixpgcj.com</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>g8eyrdtyw</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>kwsvxbqut</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>vhvyqbo@xisaoue.com</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>SQMSoKr</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>hqbqqjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>hooydrbr@ykhkhonj.com</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>QTwe5W7t</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>tuwegjnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>gmlcvgwvd@kilmuinjv.com</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>yJK5GZ91s</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>zqegwsatn</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>bpyxmfu@rblfzte.com</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>aspnmRz</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>mgeqxvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>yuqmzjlldg@pmoozqbwoo.com</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Ei7LTe2kxG</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>jyctnzbbwr</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added get by author method
</commit_message>
<xml_diff>
--- a/tests/data/registered_users.xlsx
+++ b/tests/data/registered_users.xlsx
@@ -401,7 +401,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -414,20 +414,20 @@
     <col width="20.7109375" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
-          <t>ohhwjntxqmu@smyqtdnrtkx.com</t>
+          <t>1213213</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
-          <t>EDNLX894ZDR</t>
+          <t>PuHJo0YDXT</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
-          <t>tkpjplpcxcj</t>
+          <t>ztkinrkjpk</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added check article was deleted
</commit_message>
<xml_diff>
--- a/tests/data/registered_users.xlsx
+++ b/tests/data/registered_users.xlsx
@@ -417,17 +417,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>1213213</t>
+          <t>umykwypg@wgghawuk.com</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>PuHJo0YDXT</t>
+          <t>z7ZvCZ</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>ztkinrkjpk</t>
+          <t>hlithp</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new test and dates functions
</commit_message>
<xml_diff>
--- a/tests/data/registered_users.xlsx
+++ b/tests/data/registered_users.xlsx
@@ -417,17 +417,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>vqifanad@vbtymexg.com</t>
+          <t>xmsfmlxd@rxegdqdu.com</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>AGB6C5</t>
+          <t>pufIpeu</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>znnedw</t>
+          <t>nydjdpk</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added field bio for UserRequest
</commit_message>
<xml_diff>
--- a/tests/data/registered_users.xlsx
+++ b/tests/data/registered_users.xlsx
@@ -401,7 +401,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -417,17 +417,110 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>wtpihaqo@qkdissml.com</t>
+          <t>lxmpqrh@gzcmhid.com</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>pufIpeu</t>
+          <t>zp89Pr2</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>nydjdpk</t>
+          <t>gefkqyw</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Travell</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>uytvxnsk@aheblyml.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>IO7vYRsw</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>lcldcrhi</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Software</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>rguvqduo@lssjcxvl.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>5b3RISBIY7N</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>tctiioxxlgm</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>I love to code in Py</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>dhkflsmx@mdksplfs.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>wag6JQNc</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>pdguxjge</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Foodie. </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>zhbggvvn@ybnxlseg.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>YAceJZ</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>tipuft</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Foodie. Yoga enthusi</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
New user and yml
</commit_message>
<xml_diff>
--- a/tests/data/registered_users.xlsx
+++ b/tests/data/registered_users.xlsx
@@ -401,7 +401,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -417,110 +417,550 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>bkgtogfnxx@boncpnkphe.com</t>
+          <t>zoxmqkn@xvimixw.com</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>qlgy93pucM</t>
+          <t>bRf3dxR</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>ecpeocounc</t>
+          <t>rmwidji</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Software e</t>
+          <t>Travell</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>wsjiovrw@eluyvptj.com</t>
+          <t>opfkeurslv@oxomotqawj.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>aFBA6s3Q</t>
+          <t>VqN2dT6WNP</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>udycreui</t>
+          <t>fpvjiyvtvt</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>I love t</t>
+          <t>Lifelong l</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>fqblanpgcv@ypqymnvgin.com</t>
+          <t>ktqtlhrpdyn@xjjeqjouifr.com</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>v7s0JYogAO</t>
+          <t>YmfV8xrXKbA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ykubuaynxx</t>
+          <t>xiuzmpaiojn</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">I love to </t>
+          <t>I love to c</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>xvgucssj@ispjavzn.com</t>
+          <t>fcoxxtcldvb@owrppwzrswo.com</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>bwK2qmz5</t>
+          <t>bRIc8Ep2Chr</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>kzsacfqd</t>
+          <t>rlovzeosbsk</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Lifelong</t>
+          <t>Software en</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>svkqdfvvel@iofecnkvhg.com</t>
+          <t>pejsbchtmte@rthrommxpib.com</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>bw6RgE9eEE</t>
+          <t>uR6uEok316Y</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>bgvdqigltu</t>
+          <t>dqeguqmndih</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Traveller a</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ymiumofqgsq@eiesgtbysxi.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4u0NQcTs5JJ</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>kadoejagytz</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>I love to c</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>kxkdhxomuyx@jpvkcsmxwkp.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>JuWLBXrBq59</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fxvamidadsl</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>I love to c</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ltwkmwglwi@semnuldakb.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>H1iG8OylMx</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>rzspuoiwfj</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traveller </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>tbskknfhe@rddfpzsyi.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>xiBAi6iz9</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>gvbmwvjjj</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Software </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>pyohgqw@vsteqjb.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>8FdPJEn</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>inwewdn</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Foodie.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>tczjmm@vqsmlp.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>KZ2hrP</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>qzogiv</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ziojaz@mvtoif.com</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>3IREI7</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ibuitw</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Foodie</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cyppyg@reeurc.com</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>NCBKV6</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>coipxl</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ctrwlna@ztvzuum.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Hpl6lfl</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>rvgyvnj</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Foodie.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>bncdykcxev@cbqchvwsfl.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>4cgoBdtIdd</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>baalnaprgn</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>Lifelong l</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>fcazdejoyy@zjetbmkqpg.com</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BnAQRfGnJT</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>obgrgsfgbo</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traveller </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>pzfsoa@ctqcyo.com</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1kDEdI</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>fwgmed</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Softwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>iwksmntrjn@ffyimoytpk.com</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>yu2uztCXAm</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>shwbnpkses</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Foodie. Yo</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>sjvaunm@muhlsoz.com</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>c1AzmWM</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>cnqzxkb</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love </t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>tautpgrr@bulnrzkn.com</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1ifoGNNG</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>jzgnutfs</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Foodie. </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>jcgzholj@usipwimf.com</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Qs8AeXjY</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>rfavrkxv</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Travelle</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>srmontf@sdlepvq.com</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>hpy7S4n</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>rtaxaxs</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Travell</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>cjgjwmepkj@qokiqlxynf.com</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ep0W3pdb86</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>mdjmmeqmiw</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Foodie. Yo</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>vncwqxmx@ejkwouwr.com</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>8BLzUZn3</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>csirimsz</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Travelle</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>gxnbqevc@flyrxuwa.com</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>RPGQnPQT</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>xayqiosg</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Travelle</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added script for actions
</commit_message>
<xml_diff>
--- a/tests/data/registered_users.xlsx
+++ b/tests/data/registered_users.xlsx
@@ -417,22 +417,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>nxgobpjz@cdcgaqrz.com</t>
+          <t>skfaycx@erxnbzm.com</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>NDiqcRKSBw2</t>
+          <t>H2NyiyK</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>jceghsdgfhn</t>
+          <t>qsgnucc</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Traveller and bookwo</t>
+          <t>Foodie.</t>
         </is>
       </c>
     </row>

</xml_diff>